<commit_message>
Finished readme for assignment 7
</commit_message>
<xml_diff>
--- a/Session 07/Submission/ERA V1 - Viraj - Assignment 07 - RF Calculation.xlsx
+++ b/Session 07/Submission/ERA V1 - Viraj - Assignment 07 - RF Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Root\Personal\WorkSpace\era-v1\Session 07\Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70C77E2-C2D9-429D-B473-801090C0BF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FEFBF95-A95A-4CDC-A0F3-5A27E2D3B238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B87277F1-D8E0-4270-BAC2-114CE89561B4}"/>
   </bookViews>
@@ -286,10 +286,11 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -314,14 +315,13 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,11 +449,11 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E874EB6A-C957-4579-8E33-687C596B2291}" name="Layer"/>
     <tableColumn id="2" xr3:uid="{1325CD97-6359-47FA-AC73-5186630E09F2}" name="r_in"/>
-    <tableColumn id="3" xr3:uid="{928F64D4-B500-409C-B67E-4287D353A826}" name="n_in" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{928F64D4-B500-409C-B67E-4287D353A826}" name="n_in" dataDxfId="11"/>
     <tableColumn id="4" xr3:uid="{C0929AA2-91BA-44F7-ABD0-CC1F24022D4A}" name="j_in"/>
     <tableColumn id="5" xr3:uid="{B921D946-CFC5-4362-A6ED-CD310093E0D4}" name="s"/>
     <tableColumn id="6" xr3:uid="{D9FF0FF2-35EA-4DDD-885B-A1A94B68A80B}" name="r_out"/>
-    <tableColumn id="7" xr3:uid="{93AC1FE6-69F0-4B2B-8498-812BC46649FA}" name="n_out" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{93AC1FE6-69F0-4B2B-8498-812BC46649FA}" name="n_out" dataDxfId="10"/>
     <tableColumn id="8" xr3:uid="{FBA2762A-465E-4654-B543-1600C46F4A4E}" name="j_out"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -461,31 +461,31 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB216C57-85C8-4560-B5AF-B03B493FAD08}" name="Table1" displayName="Table1" ref="B26:I34" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB216C57-85C8-4560-B5AF-B03B493FAD08}" name="Table1" displayName="Table1" ref="B26:I34" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="B26:I34" xr:uid="{DB216C57-85C8-4560-B5AF-B03B493FAD08}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{6CE3C1F0-822D-46D6-9D4F-1E97EBD66D21}" name="Layer" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{6CE3C1F0-822D-46D6-9D4F-1E97EBD66D21}" name="Layer" dataDxfId="7">
       <calculatedColumnFormula>A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{4BCDA8B8-15BA-4119-BB09-CFE5BCB01DA1}" name="r_in" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{4BCDA8B8-15BA-4119-BB09-CFE5BCB01DA1}" name="r_in" dataDxfId="6">
       <calculatedColumnFormula>C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B40DA856-6ADA-44E1-B23F-F94788E2E2E3}" name="n_in" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{B40DA856-6ADA-44E1-B23F-F94788E2E2E3}" name="n_in" dataDxfId="5">
       <calculatedColumnFormula>B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{7C38AE21-044F-4256-896B-B6034C9CA8EF}" name="j_in" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{7C38AE21-044F-4256-896B-B6034C9CA8EF}" name="j_in" dataDxfId="4">
       <calculatedColumnFormula>G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{EF6D6A5D-3461-4D0C-8C6C-6B3E8C8884A3}" name="s" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{EF6D6A5D-3461-4D0C-8C6C-6B3E8C8884A3}" name="s" dataDxfId="3">
       <calculatedColumnFormula>F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{6E88AB2A-0A71-4F38-9603-B70EE87F8E8A}" name="r_out" dataDxfId="6">
+    <tableColumn id="6" xr3:uid="{6E88AB2A-0A71-4F38-9603-B70EE87F8E8A}" name="r_out" dataDxfId="2">
       <calculatedColumnFormula>J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D15DF32A-57AF-405F-BE20-BCE9B4329836}" name="n_out" dataDxfId="5">
+    <tableColumn id="7" xr3:uid="{D15DF32A-57AF-405F-BE20-BCE9B4329836}" name="n_out" dataDxfId="1">
       <calculatedColumnFormula>I2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{52562617-BC96-4C7F-AE76-104C47DFB60B}" name="j_out" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{52562617-BC96-4C7F-AE76-104C47DFB60B}" name="j_out" dataDxfId="0">
       <calculatedColumnFormula>H2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BD6788-01C6-4727-A14C-1F3F18C7D73D}">
   <dimension ref="B2:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H8" si="0">G2*F2</f>
+        <f t="shared" ref="H2:H7" si="0">G2*F2</f>
         <v>1</v>
       </c>
       <c r="I2" s="6">
@@ -1126,7 +1126,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="4">
-        <f t="shared" ref="J2:J8" si="1">C2+(D2-1)*G2</f>
+        <f t="shared" ref="J2:J7" si="1">C2+(D2-1)*G2</f>
         <v>3</v>
       </c>
     </row>
@@ -1135,7 +1135,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="8">
-        <f t="shared" ref="B3:C8" si="2">IFERROR(I2,"")</f>
+        <f t="shared" ref="B3:C7" si="2">IFERROR(I2,"")</f>
         <v>28</v>
       </c>
       <c r="C3" s="5">
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G8" si="3">IFERROR(H2,"")</f>
+        <f t="shared" ref="G3:G7" si="3">IFERROR(H2,"")</f>
         <v>1</v>
       </c>
       <c r="H3" s="3">
@@ -1601,35 +1601,35 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="str">
-        <f t="shared" ref="B28:B35" si="10">A3</f>
+        <f t="shared" ref="B28:B34" si="10">A3</f>
         <v>Conv2d</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ref="C28:C35" si="11">C3</f>
+        <f t="shared" ref="C28:C34" si="11">C3</f>
         <v>3</v>
       </c>
       <c r="D28" s="17">
-        <f t="shared" ref="D28:D35" si="12">B3</f>
+        <f t="shared" ref="D28:D34" si="12">B3</f>
         <v>28</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ref="E28:E35" si="13">G3</f>
+        <f t="shared" ref="E28:E34" si="13">G3</f>
         <v>1</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" ref="F28:F35" si="14">F3</f>
+        <f t="shared" ref="F28:F34" si="14">F3</f>
         <v>1</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" ref="G28:G35" si="15">J3</f>
+        <f t="shared" ref="G28:G34" si="15">J3</f>
         <v>5</v>
       </c>
       <c r="H28" s="17">
-        <f t="shared" ref="H28:H35" si="16">I3</f>
+        <f t="shared" ref="H28:H34" si="16">I3</f>
         <v>26</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" ref="I28:I35" si="17">H3</f>
+        <f t="shared" ref="I28:I34" si="17">H3</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>